<commit_message>
create reactome pathway png for pre_replication proteins
</commit_message>
<xml_diff>
--- a/PTEN/Step_3_trans_effect/csv/Reactome_cell_cycle.xlsx
+++ b/PTEN/Step_3_trans_effect/csv/Reactome_cell_cycle.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brittany henderson\GitHub\WhenMutationsDontMatter\PTEN\Step_3_trans_effect\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C769E2-264B-49B7-AB0B-8293EC9F0A38}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E844005-646E-4CBA-8FEA-9C036B19837C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{A4A76A2A-01DD-4CD7-BFD1-431697823A18}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" activeTab="1" xr2:uid="{A4A76A2A-01DD-4CD7-BFD1-431697823A18}"/>
   </bookViews>
   <sheets>
     <sheet name="cell_cycle" sheetId="1" r:id="rId1"/>
-    <sheet name="g1_to_s" sheetId="2" r:id="rId2"/>
+    <sheet name="pre_replication" sheetId="3" r:id="rId2"/>
+    <sheet name="g1_to_s" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="683">
   <si>
     <t>REACTOME_CELL_CYCLE</t>
   </si>
@@ -2078,6 +2079,9 @@
   </si>
   <si>
     <t>TK2</t>
+  </si>
+  <si>
+    <t>pre_replication</t>
   </si>
 </sst>
 </file>
@@ -2434,7 +2438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6BA0D98-08C7-4CF9-A848-56D5076EABB9}">
   <dimension ref="A1:YZ1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -4476,6 +4480,191 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920F795D-CD7A-45A7-888B-50187C794EED}">
+  <dimension ref="A1:A34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>457</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{442AD71C-64AD-443E-B84C-F7215F4AEEE9}">
   <dimension ref="A1:DG1"/>
   <sheetViews>

</xml_diff>